<commit_message>
SQL DUMP 6.0 (FINAL)
-Finalised Commands Document
-Finalised Database Template
-Finalised SQL Dump
</commit_message>
<xml_diff>
--- a/SQL Database Template.xlsx
+++ b/SQL Database Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6751F5AD-1984-4B5F-B249-5934A5C2F3B6}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290231B7-1F4F-49EB-959B-D26F7BCF2487}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="4872" windowHeight="7068" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>LANGUAGES</t>
   </si>
@@ -106,16 +106,39 @@
   </si>
   <si>
     <t>PRIMARY KEY</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Luke@l.com</t>
+  </si>
+  <si>
+    <t>Mitch@m.com</t>
+  </si>
+  <si>
+    <t>Ryan@r.com</t>
+  </si>
+  <si>
+    <t>Gearoid@g.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -141,7 +164,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -273,11 +296,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -291,13 +337,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -576,39 +626,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A7:O27"/>
+  <dimension ref="A7:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.77734375" customWidth="1"/>
-    <col min="2" max="4" width="15.77734375" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.44140625" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="5" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
     <col min="8" max="9" width="18" customWidth="1"/>
     <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B8" s="16" t="s">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B8" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B10" s="17" t="s">
+    <row r="9" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="16" t="s">
         <v>25</v>
       </c>
       <c r="D10" s="5" t="s">
@@ -619,13 +669,14 @@
         <v>19</v>
       </c>
       <c r="H10" s="6"/>
-      <c r="I10" s="11"/>
+      <c r="I10" s="6"/>
       <c r="N10" s="5" t="s">
         <v>20</v>
       </c>
       <c r="O10" s="6"/>
-    </row>
-    <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P10" s="6"/>
+    </row>
+    <row r="11" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D11" s="10" t="s">
         <v>1</v>
       </c>
@@ -638,15 +689,20 @@
       <c r="H11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="11"/>
+      <c r="I11" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="N11" s="10" t="s">
         <v>11</v>
       </c>
       <c r="O11" s="7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P11" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D12" s="8">
         <v>1</v>
       </c>
@@ -659,15 +715,20 @@
       <c r="H12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="11"/>
+      <c r="I12" s="17" t="s">
+        <v>28</v>
+      </c>
       <c r="N12" s="2">
         <v>1</v>
       </c>
       <c r="O12" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P12" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D13" s="9">
         <v>2</v>
       </c>
@@ -680,15 +741,20 @@
       <c r="H13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I13" s="11"/>
+      <c r="I13" s="18" t="s">
+        <v>29</v>
+      </c>
       <c r="N13" s="1">
         <v>2</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P13" s="18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D14" s="9">
         <v>3</v>
       </c>
@@ -701,25 +767,33 @@
       <c r="H14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="11"/>
+      <c r="I14" s="18" t="s">
+        <v>30</v>
+      </c>
       <c r="N14" s="1">
         <v>3</v>
       </c>
       <c r="O14" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P14" s="19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="G15" s="1">
         <v>4</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I15" s="11"/>
-    </row>
-    <row r="16" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="17" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="I15" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="P15" s="20"/>
+    </row>
+    <row r="16" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E17" s="5" t="s">
         <v>18</v>
       </c>
@@ -733,23 +807,23 @@
       <c r="L17" s="6"/>
       <c r="M17" s="3"/>
     </row>
-    <row r="18" spans="5:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E18" s="13" t="s">
+    <row r="18" spans="5:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="13" t="s">
+      <c r="F18" s="10" t="s">
         <v>1</v>
       </c>
       <c r="H18" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="I18" s="14" t="s">
+      <c r="I18" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="J18" s="15" t="s">
+      <c r="J18" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="K18" s="15" t="s">
+      <c r="K18" s="14" t="s">
         <v>24</v>
       </c>
       <c r="L18" s="7" t="s">
@@ -759,7 +833,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E19" s="2">
         <v>1</v>
       </c>
@@ -781,7 +855,7 @@
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
     </row>
-    <row r="20" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E20" s="2">
         <v>1</v>
       </c>
@@ -803,7 +877,7 @@
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
     </row>
-    <row r="21" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E21" s="1">
         <v>2</v>
       </c>
@@ -825,7 +899,7 @@
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
     </row>
-    <row r="22" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E22" s="1">
         <v>3</v>
       </c>
@@ -847,7 +921,7 @@
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
     </row>
-    <row r="23" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E23" s="1">
         <v>4</v>
       </c>
@@ -869,7 +943,7 @@
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
     </row>
-    <row r="24" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E24" s="1">
         <v>5</v>
       </c>
@@ -891,7 +965,7 @@
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
     </row>
-    <row r="25" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E25" s="1">
         <v>6</v>
       </c>
@@ -913,7 +987,7 @@
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
     </row>
-    <row r="26" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E26" s="1">
         <v>7</v>
       </c>
@@ -935,7 +1009,7 @@
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
     </row>
-    <row r="27" spans="5:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E27" s="1">
         <v>8</v>
       </c>
@@ -958,6 +1032,15 @@
       <c r="M27" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I12" r:id="rId1" xr:uid="{6D77C1B8-AAEA-4D54-BFD7-C21B5A37702C}"/>
+    <hyperlink ref="I13" r:id="rId2" xr:uid="{14215347-5784-40EF-956C-6FFB350599BB}"/>
+    <hyperlink ref="I14" r:id="rId3" xr:uid="{1FE4D426-D0CE-4BDB-84F6-8DBBE7B52289}"/>
+    <hyperlink ref="I15" r:id="rId4" xr:uid="{C3E8A56E-CACF-4F0E-BE9A-BAAAD6E62A0F}"/>
+    <hyperlink ref="P12" r:id="rId5" xr:uid="{CF5A4725-0C4A-427C-99DF-86F59AC0473E}"/>
+    <hyperlink ref="P13" r:id="rId6" xr:uid="{FB990CFF-A720-494D-B2F9-919F30F42B1C}"/>
+    <hyperlink ref="P14" r:id="rId7" xr:uid="{F175DF85-8A7E-471A-96B3-997F497E18A8}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>